<commit_message>
This file replaced the User Reqmt Prioritization.xlsx file
</commit_message>
<xml_diff>
--- a/System Requirements List.xlsx
+++ b/System Requirements List.xlsx
@@ -133,10 +133,10 @@
     </r>
   </si>
   <si>
-    <t>Each site page shall use relevant articles written in darker font and displayed next to their corresponding photos.  Currently, photos are placed on a page without corresponding label or reference.  Light font is used on a light gray background which is hard to read.</t>
-  </si>
-  <si>
     <t>Each page shall use consistent line spacing, font size and bold-type font:  double line-spacing between paragraphs, after page titles, and after subheadings; 26pt bold font for page titles and 20pt bold font for subheadings.  Currently, some pages have inconsistent formatting.</t>
+  </si>
+  <si>
+    <t>Each site page shall use relevant articles typed in darker font with higher contrast and displayed next to their corresponding photos.  Currently, photos are placed on a page without corresponding label or reference.  Light font is used on a light gray background which can be difficult to read.</t>
   </si>
 </sst>
 </file>
@@ -259,14 +259,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -768,24 +768,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
@@ -833,11 +833,11 @@
       <c r="D5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -850,8 +850,8 @@
       <c r="D6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -863,8 +863,8 @@
       <c r="D7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" s="2" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -879,8 +879,8 @@
       <c r="D8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" ht="63" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -892,8 +892,8 @@
       <c r="D9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -908,8 +908,8 @@
       <c r="D10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" s="2" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -924,8 +924,8 @@
       <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" s="2" customFormat="1" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">

</xml_diff>

<commit_message>
This file replaced the User Reqmt Prioritization file
</commit_message>
<xml_diff>
--- a/System Requirements List.xlsx
+++ b/System Requirements List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Assigned to</t>
   </si>
@@ -133,10 +133,13 @@
     </r>
   </si>
   <si>
-    <t>Each page shall use consistent line spacing, font size and bold-type font:  double line-spacing between paragraphs, after page titles, and after subheadings; 26pt bold font for page titles and 20pt bold font for subheadings.  Currently, some pages have inconsistent formatting.</t>
-  </si>
-  <si>
-    <t>Each site page shall use relevant articles typed in darker font with higher contrast and displayed next to their corresponding photos.  Currently, photos are placed on a page without corresponding label or reference.  Light font is used on a light gray background which can be difficult to read.</t>
+    <t>Each site page shall use relevant articles typed in darker font with higher contrast background &amp; displayed next to their corresponding photos.  Currently, photos are placed on a page without corresponding label or reference except when hovering over photos.  Light font is used on a light gray background which can be difficult to read.</t>
+  </si>
+  <si>
+    <t>Website Pages (Content presentation)</t>
+  </si>
+  <si>
+    <t>Each page shall use consistent line spacing, font type/size, and bold-type font that provides better user experience:  double-line spacing between paragraphs, after page titles, and after subheadings; 26pt bold font for page titles and 20pt bold font for subheadings.  Currently, some pages have inconsistent formatting.</t>
   </si>
 </sst>
 </file>
@@ -753,18 +756,20 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="53.5703125" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -820,12 +825,12 @@
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="189" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>9</v>
@@ -834,10 +839,10 @@
         <v>20</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="63" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added mobile formatting requirements
</commit_message>
<xml_diff>
--- a/System Requirements List.xlsx
+++ b/System Requirements List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac185235\Documents\GitHub\MIST7590-Smithgall-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenelazo\Documents\GitHub\MIST7590-Smithgall-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>Assigned to</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Details should be provided for each location such as different attractions, land marks, trails, etc. These details may help the user refine their search based on what they are wanting to see</t>
+  </si>
+  <si>
+    <t>Application menu will be formatted for mobile browsers using Bootstrap for ease of viewing and item selection.</t>
+  </si>
+  <si>
+    <t>Application forms will be formatted for mobile browsers using Bootstrap to make data entry easier, including reducing the amount of typing required versus tapping to select an item.</t>
   </si>
 </sst>
 </file>
@@ -827,7 +833,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,7 +998,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1005,8 +1011,12 @@
       <c r="D11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="E11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:6" s="2" customFormat="1" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">

</xml_diff>